<commit_message>
update HR and CI
</commit_message>
<xml_diff>
--- a/data/RaccoonLikelyhoodLarvaeInJar/all500cox_coeff_HR_CI_122721.xlsx
+++ b/data/RaccoonLikelyhoodLarvaeInJar/all500cox_coeff_HR_CI_122721.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lindsay\Dropbox\Raccoon\larvae\oyster\larvae survival stats\GitHub\RaccoonOlyLarvalSurvival2\data\RaccoonLikelyhoodLarvaeInJar\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lalma\Dropbox\Raccoon\larvae\oyster\larvae survival stats\GitHub\RaccoonOlyLarvalSurvival2\data\RaccoonLikelyhoodLarvaeInJar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F224E546-04CE-4655-AE32-0B416F1E3CDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B279BCEF-123B-4076-A390-5A6086B5EC0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{364C95DC-FF29-4104-B9BF-EAA6328331F2}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{364C95DC-FF29-4104-B9BF-EAA6328331F2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -43,12 +43,6 @@
     <t>treatment</t>
   </si>
   <si>
-    <t>by</t>
-  </si>
-  <si>
-    <t>mean</t>
-  </si>
-  <si>
     <t>CI20</t>
   </si>
   <si>
@@ -91,21 +85,35 @@
     <t>coefficients_PW5ref</t>
   </si>
   <si>
-    <t>data</t>
-  </si>
-  <si>
     <t>0.025quantile</t>
   </si>
   <si>
     <t>0.975quantile</t>
+  </si>
+  <si>
+    <t>mean_expectedHR</t>
+  </si>
+  <si>
+    <t>datafrom</t>
+  </si>
+  <si>
+    <t>interaction</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -133,7 +141,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -144,6 +152,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -462,64 +476,70 @@
   <dimension ref="A1:I28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="5" width="8.7265625" style="1"/>
-    <col min="6" max="6" width="8.7265625" style="2"/>
-    <col min="7" max="7" width="14.1796875" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="8.7265625" style="3"/>
+    <col min="1" max="1" width="8.77734375" style="1"/>
+    <col min="2" max="2" width="9.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.77734375" style="1"/>
+    <col min="5" max="5" width="9.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.21875" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.44140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="8.77734375" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
+      <c r="B2" s="1">
+        <v>14</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="1">
+        <v>20</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>4</v>
-      </c>
-      <c r="B2" s="1">
-        <v>14</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" s="1">
-        <v>20</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>6</v>
       </c>
       <c r="G2" s="1">
         <v>-0.84611559999999997</v>
@@ -531,24 +551,24 @@
         <v>-0.61310469999999995</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1">
+        <v>14</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="1">
+        <v>14</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>4</v>
-      </c>
-      <c r="B3" s="1">
-        <v>14</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" s="1">
-        <v>14</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>6</v>
       </c>
       <c r="G3" s="1">
         <v>-0.12113518</v>
@@ -560,24 +580,24 @@
         <v>6.9245189999999998E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1">
+        <v>14</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="1">
+        <v>14</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>4</v>
-      </c>
-      <c r="B4" s="1">
-        <v>14</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" s="1">
-        <v>14</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>6</v>
       </c>
       <c r="G4" s="1">
         <v>-0.76846559999999997</v>
@@ -589,24 +609,24 @@
         <v>-0.54680410000000002</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="1">
+        <v>14</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="1">
+        <v>14</v>
+      </c>
+      <c r="F5" s="2" t="s">
         <v>4</v>
-      </c>
-      <c r="B5" s="1">
-        <v>14</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" s="1">
-        <v>14</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>6</v>
       </c>
       <c r="G5" s="1">
         <v>-0.51838039999999996</v>
@@ -618,24 +638,24 @@
         <v>-0.35790359999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="1">
+        <v>14</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="1">
+        <v>20</v>
+      </c>
+      <c r="F6" s="2" t="s">
         <v>4</v>
-      </c>
-      <c r="B6" s="1">
-        <v>14</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" s="1">
-        <v>20</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>6</v>
       </c>
       <c r="G6" s="1">
         <v>-5.0255830000000001E-2</v>
@@ -647,24 +667,24 @@
         <v>0.26152502</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="1">
+        <v>14</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" s="1">
+        <v>20</v>
+      </c>
+      <c r="F7" s="2" t="s">
         <v>4</v>
-      </c>
-      <c r="B7" s="1">
-        <v>14</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E7" s="1">
-        <v>20</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>6</v>
       </c>
       <c r="G7" s="1">
         <v>0.12712209999999999</v>
@@ -676,24 +696,24 @@
         <v>0.4157651</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="1">
+        <v>14</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="1">
+        <v>20</v>
+      </c>
+      <c r="F8" s="2" t="s">
         <v>4</v>
-      </c>
-      <c r="B8" s="1">
-        <v>14</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E8" s="1">
-        <v>20</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>6</v>
       </c>
       <c r="G8" s="1">
         <v>-0.12257220000000001</v>
@@ -705,24 +725,24 @@
         <v>0.17649239999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B9" s="1">
         <v>20</v>
       </c>
       <c r="C9" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>7</v>
-      </c>
       <c r="E9" s="1">
         <v>14</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G9" s="1">
         <v>0.45428079999999998</v>
@@ -734,24 +754,24 @@
         <v>0.67886409999999997</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B10" s="1">
         <v>20</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E10" s="1">
+        <v>14</v>
+      </c>
+      <c r="F10" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="E10" s="1">
-        <v>14</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>10</v>
       </c>
       <c r="G10" s="1">
         <v>-0.18461562000000001</v>
@@ -763,24 +783,24 @@
         <v>6.8488950000000007E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B11" s="1">
         <v>20</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E11" s="1">
         <v>14</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G11" s="1">
         <v>3.9518320000000003E-2</v>
@@ -792,24 +812,24 @@
         <v>0.25459977</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B12" s="1">
         <v>20</v>
       </c>
       <c r="C12" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D12" s="1" t="s">
-        <v>7</v>
-      </c>
       <c r="E12" s="1">
         <v>20</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G12" s="1">
         <v>0.301977</v>
@@ -821,24 +841,24 @@
         <v>0.49463259999999998</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B13" s="1">
         <v>20</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E13" s="1">
         <v>20</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G13" s="1">
         <v>-0.26092664999999998</v>
@@ -850,24 +870,24 @@
         <v>-3.0091420000000001E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B14" s="1">
         <v>20</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D14" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E14" s="1">
+        <v>20</v>
+      </c>
+      <c r="F14" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="E14" s="1">
-        <v>20</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>11</v>
       </c>
       <c r="G14" s="1">
         <v>-0.17143685</v>
@@ -879,24 +899,24 @@
         <v>3.1122259999999999E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B15" s="1">
         <v>14</v>
       </c>
       <c r="C15" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D15" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D15" s="1" t="s">
-        <v>7</v>
-      </c>
       <c r="E15" s="1">
         <v>20</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G15" s="1">
         <v>-0.55202910000000005</v>
@@ -908,24 +928,24 @@
         <v>-0.342337</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B16" s="1">
         <v>14</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E16" s="1">
         <v>14</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G16" s="1">
         <v>-0.82235970000000003</v>
@@ -937,24 +957,24 @@
         <v>-0.60179879999999997</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17" s="1">
+        <v>14</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B17" s="1">
-        <v>14</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="E17" s="1">
         <v>14</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G17" s="1">
         <v>-0.60836239999999997</v>
@@ -966,24 +986,24 @@
         <v>-0.41715819999999998</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B18" s="1">
         <v>14</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E18" s="1">
         <v>20</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G18" s="1">
         <v>-0.38825049</v>
@@ -995,24 +1015,24 @@
         <v>-8.8289969999999995E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B19" s="1">
+        <v>14</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B19" s="1">
-        <v>14</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="E19" s="1">
         <v>20</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G19" s="1">
         <v>-0.52311702000000004</v>
@@ -1024,24 +1044,24 @@
         <v>-0.24693159000000001</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B20" s="1">
         <v>20</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E20" s="1">
         <v>14</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G20" s="4">
         <f>-0.4980607</f>
@@ -1054,24 +1074,24 @@
         <v>-0.26571289999999997</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B21" s="1">
+        <v>20</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D21" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B21" s="1">
-        <v>20</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="E21" s="1">
         <v>14</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G21" s="1">
         <v>-0.28873144000000001</v>
@@ -1083,24 +1103,24 @@
         <v>-7.5783349999999999E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B22" s="1">
         <v>20</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E22" s="1">
         <v>20</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G22" s="1">
         <f>-0.7029296</f>
@@ -1113,24 +1133,24 @@
         <v>-0.45354220000000001</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B23" s="1">
+        <v>20</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D23" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B23" s="1">
-        <v>20</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="E23" s="1">
         <v>20</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G23" s="1">
         <f>-0.7259525</f>
@@ -1143,24 +1163,24 @@
         <v>-0.50397959999999997</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B24" s="1">
         <v>14</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E24" s="1">
         <v>20</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G24" s="1">
         <v>-0.42307686999999999</v>
@@ -1172,24 +1192,24 @@
         <v>-0.19964401000000001</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B25" s="1">
         <v>14</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E25" s="1">
         <v>20</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G25" s="1">
         <v>-0.52311702000000004</v>
@@ -1201,24 +1221,24 @@
         <v>-0.24693159000000001</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B26" s="1">
         <v>14</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E26" s="1">
         <v>14</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G26" s="1">
         <v>-2.8983020000000002E-3</v>
@@ -1230,24 +1250,24 @@
         <v>0.20109299999999999</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B27" s="1">
         <v>20</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E27" s="1">
         <v>20</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="G27" s="1">
         <v>-0.27614717999999999</v>
@@ -1259,24 +1279,24 @@
         <v>-4.5098890000000003E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B28" s="1">
         <v>14</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E28" s="1">
         <v>20</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G28" s="1">
         <f>-0.69782</f>

</xml_diff>